<commit_message>
Scrubbed BOM for obsolete parts
</commit_message>
<xml_diff>
--- a/BOM/PREP400-BOM.xlsx
+++ b/BOM/PREP400-BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boniface\Documents\GitHub\PCB\Projects\PREP400\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boniface\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F011BB9D-06D8-4A73-A9F8-7FAA7DA136E6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="4548"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="4548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backflow" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="278">
   <si>
     <t>J1</t>
   </si>
@@ -27,9 +28,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>Ref. Des.</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -93,9 +91,6 @@
     <t>C2012X5R0J476M125AC</t>
   </si>
   <si>
-    <t>1276-1852-1-ND</t>
-  </si>
-  <si>
     <t>1276-6600-1-ND</t>
   </si>
   <si>
@@ -117,15 +112,9 @@
     <t>DIODE SCHOTTKY 30V 200MA SOT23-3</t>
   </si>
   <si>
-    <t>Fairchild</t>
-  </si>
-  <si>
     <t>BAT54</t>
   </si>
   <si>
-    <t>BAT54FSCT-ND</t>
-  </si>
-  <si>
     <t>BAT54-FDICT-ND</t>
   </si>
   <si>
@@ -138,9 +127,6 @@
     <t>BZX84C3V3</t>
   </si>
   <si>
-    <t>BZX84C3V3FSCT-ND</t>
-  </si>
-  <si>
     <t>BZX84C3V3LT1GOSCT-ND</t>
   </si>
   <si>
@@ -156,9 +142,6 @@
     <t>BAT54S</t>
   </si>
   <si>
-    <t>BAT54SFSCT-ND</t>
-  </si>
-  <si>
     <t>BAT54S-FDICT-ND</t>
   </si>
   <si>
@@ -171,9 +154,6 @@
     <t>BAV99</t>
   </si>
   <si>
-    <t>BAV99FSCT-ND</t>
-  </si>
-  <si>
     <t>1727-4311-1-ND</t>
   </si>
   <si>
@@ -192,9 +172,6 @@
     <t>480-6445-ND</t>
   </si>
   <si>
-    <t>480-5530-ND</t>
-  </si>
-  <si>
     <t>IC5, IC6, IC7, IC8, IC11, IC12, IC13, IC14</t>
   </si>
   <si>
@@ -270,9 +247,6 @@
     <t>R4, R6, R8, R10</t>
   </si>
   <si>
-    <t>Yageo</t>
-  </si>
-  <si>
     <t>D15, D16, D17, D18, D27, D28, D29, D30</t>
   </si>
   <si>
@@ -339,9 +313,6 @@
     <t>445-5666-1-ND</t>
   </si>
   <si>
-    <t>311-1344-1-ND</t>
-  </si>
-  <si>
     <t>CAP CER 10000PF 50V X7R 0603</t>
   </si>
   <si>
@@ -405,9 +376,6 @@
     <t>RC1608F102CS</t>
   </si>
   <si>
-    <t>1276-3484-1-ND</t>
-  </si>
-  <si>
     <t>RES SMD 39K OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -534,9 +502,6 @@
     <t>36-5006-ND</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32, TP33, TP34, TP35, TP36, TP37, TP38, TP39, TP40, TP41, TP42, TP43, TP44, TP45, TP46, TP47, TP478, TP49, TP50, TP51, TP52, TP53, TP54, TP55, TP56</t>
-  </si>
-  <si>
     <t>TP19, TP20, TP21, TP22</t>
   </si>
   <si>
@@ -636,9 +601,6 @@
     <t>S9337-ND</t>
   </si>
   <si>
-    <t>Jumper</t>
-  </si>
-  <si>
     <t>Jumper Header</t>
   </si>
   <si>
@@ -738,12 +700,6 @@
     <t>CR0603-FX-1003HLFCT-ND</t>
   </si>
   <si>
-    <t>CR0603-FX-1001ELFCT-ND</t>
-  </si>
-  <si>
-    <t>YAG3603CT-ND</t>
-  </si>
-  <si>
     <t>Harwin</t>
   </si>
   <si>
@@ -766,12 +722,152 @@
   </si>
   <si>
     <t>S7078-ND</t>
+  </si>
+  <si>
+    <t>1276-1852-1-ND,
+732-7617-1-ND</t>
+  </si>
+  <si>
+    <t>BAT54FSCT-ND end of life</t>
+  </si>
+  <si>
+    <t>BAT54E6327HTSA1</t>
+  </si>
+  <si>
+    <t>BZX84C3V3FSCT-ND obsolete</t>
+  </si>
+  <si>
+    <t>BZX84C3V3-TPMSCT-ND</t>
+  </si>
+  <si>
+    <t>BAT54SFSCT-ND end of life</t>
+  </si>
+  <si>
+    <t>BAT54SLT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>BAV99FSCT-ND end of life</t>
+  </si>
+  <si>
+    <t>BAV99RFGCT-ND</t>
+  </si>
+  <si>
+    <t>P39.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>480-5530-ND is possible alternate at 5psi but would require firmware update.</t>
+  </si>
+  <si>
+    <t>NXP</t>
+  </si>
+  <si>
+    <t>FREEDOM BOARD KINETIS L</t>
+  </si>
+  <si>
+    <t>FRDM-KL25Z</t>
+  </si>
+  <si>
+    <t>FRDM-KL25Z-ND</t>
+  </si>
+  <si>
+    <t>Motherboard. Remove D8, D11 from FRDM-KL25Z</t>
+  </si>
+  <si>
+    <t>67996-212HLF</t>
+  </si>
+  <si>
+    <t>609-3213-ND</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>CONN HEADER 12POS .100 STR 15AU</t>
+  </si>
+  <si>
+    <t>Goes to J10 of FRDM-KL25Z</t>
+  </si>
+  <si>
+    <t>67996-216HLF</t>
+  </si>
+  <si>
+    <t>609-3389-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER 16POS .100 STR 15AU</t>
+  </si>
+  <si>
+    <t>Goes to J1, J9 of FRDM-KL25Z</t>
+  </si>
+  <si>
+    <t>Goes to J2 of FRDM-KL25Z</t>
+  </si>
+  <si>
+    <t>609-3214-ND</t>
+  </si>
+  <si>
+    <t>67996-220HLF</t>
+  </si>
+  <si>
+    <t>CONN HEADER 20POS .100 STR 15AU</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>609-3204-ND,
+609-3219-ND</t>
+  </si>
+  <si>
+    <t>609-3205-ND,
+609-3220-ND</t>
+  </si>
+  <si>
+    <t>609-3206-ND,
+609-3221-ND</t>
+  </si>
+  <si>
+    <t>Reference Designator</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32, TP33, TP34, TP35, TP36, TP37, TP38, TP39, TP40, TP41, TP42, TP43, TP44, TP45, TP46, TP47, TP48, TP49, TP50, TP51, TP52, TP53, TP54, TP55, TP56</t>
+  </si>
+  <si>
+    <t>311-1344-1-ND,
+490-10901-1-ND,
+478-6343-1-ND,
+709-1161-6-ND</t>
+  </si>
+  <si>
+    <t>Diodes Inc.</t>
+  </si>
+  <si>
+    <t>Micro Commercial</t>
+  </si>
+  <si>
+    <t>ON Semi</t>
+  </si>
+  <si>
+    <t>Taiwan Semi</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>1276-3484-1-ND,
+CR0603-FX-1001ELFCT-ND</t>
+  </si>
+  <si>
+    <t>P1.00KHCT-ND</t>
+  </si>
+  <si>
+    <t>Jumper - populate on header</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -921,7 +1017,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1101,8 +1197,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1253,17 +1355,6 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1323,7 +1414,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1362,7 +1453,7 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1374,8 +1465,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1383,7 +1480,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1706,977 +1806,1213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.44140625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="195.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="16">
+        <v>84</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="16">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="16">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="16">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="195.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="16">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="237" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="16">
+        <v>77</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="16">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="16">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="16">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="16">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="16">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="16">
+        <v>8</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="16">
         <v>12</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:8" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="C17" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="F17" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="16">
+        <v>4</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="16">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="D19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="E19" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="F19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="G19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="B20" s="16">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+      <c r="D20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="F20" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="16">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="16">
+        <v>8</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="16">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="16">
+        <v>8</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="G24" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="16">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="16">
+        <v>12</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="16">
+        <v>12</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="16">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="16">
+        <v>11</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="16">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="16">
+        <v>7</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="D31" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="16">
+        <v>7</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="16">
+        <v>13</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="16">
+        <v>24</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="16">
+        <v>4</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="16">
+        <v>12</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="16">
+        <v>12</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="16">
+        <v>2</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="16">
+        <v>2</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" s="16">
+        <v>52</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="E40" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="F40" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="9" t="s">
+      <c r="G40" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="19">
+        <v>4</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="16">
+        <v>1</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F30" s="6" t="s">
+      <c r="H42" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="23"/>
+      <c r="B43" s="16">
+        <v>2</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="6" t="s">
+      <c r="H43" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="23"/>
+      <c r="B44" s="16">
+        <v>1</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G44" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F41" s="6" t="s">
+      <c r="H44" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="24"/>
+      <c r="B45" s="16">
+        <v>1</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="G41" s="5"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="17" t="s">
+      <c r="E45" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="H45" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="24"/>
+      <c r="B46" s="16">
         <v>1</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-      <c r="B43" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>102</v>
+      <c r="C46" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="24"/>
+      <c r="B47" s="16">
+        <v>2</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="24"/>
+      <c r="B48" s="16">
+        <v>1</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A42:A44"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A42:A48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added expansion connector for Genesis Aux PCB
</commit_message>
<xml_diff>
--- a/BOM/PREP400-BOM.xlsx
+++ b/BOM/PREP400-BOM.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boniface\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boniface\Documents\GitHub\PCB\Projects\PREP400\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F011BB9D-06D8-4A73-A9F8-7FAA7DA136E6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B19CA4-B13E-494A-A64D-BB4B6F006B07}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="4548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backflow" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="277">
   <si>
     <t>J1</t>
   </si>
@@ -85,9 +85,6 @@
     <t>445-7492-1-ND</t>
   </si>
   <si>
-    <t>1276-1038-1-ND</t>
-  </si>
-  <si>
     <t>C2012X5R0J476M125AC</t>
   </si>
   <si>
@@ -286,15 +283,6 @@
     <t>S6106-ND</t>
   </si>
   <si>
-    <t>CONN HEADER FMAL 22PS.1" DL GOLD</t>
-  </si>
-  <si>
-    <t>PPPC112LFBN-RC</t>
-  </si>
-  <si>
-    <t>S7114-ND</t>
-  </si>
-  <si>
     <t>Goes to 12 position header of U1 (Mate: 609-3213-ND)</t>
   </si>
   <si>
@@ -532,9 +520,6 @@
     <t>Do Not Populate: C136</t>
   </si>
   <si>
-    <t>Do Not Populate: P1</t>
-  </si>
-  <si>
     <t>CAP CER 0.1UF 100V X7R 1206</t>
   </si>
   <si>
@@ -677,9 +662,6 @@
   </si>
   <si>
     <t>445-172904-1-ND</t>
-  </si>
-  <si>
-    <t>S7079-ND</t>
   </si>
   <si>
     <t>FDT86106LZCT-ND</t>
@@ -862,6 +844,22 @@
   </si>
   <si>
     <t>Jumper - populate on header</t>
+  </si>
+  <si>
+    <t>445-7486-1-ND,
+1276-1038-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	.025" BOARD SPACERS</t>
+  </si>
+  <si>
+    <t>DW-11-11-F-D-665</t>
+  </si>
+  <si>
+    <t>DW-11-11-F-D-665-ND</t>
+  </si>
+  <si>
+    <t>Not stocked. Long lead time component.</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1412,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1473,6 +1471,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1809,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1820,16 +1821,17 @@
     <col min="3" max="3" width="33.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.21875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.44140625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -1852,55 +1854,55 @@
     </row>
     <row r="2" spans="1:9" ht="195.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B2" s="16">
         <v>84</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B3" s="16">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1911,19 +1913,19 @@
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="H4" s="5"/>
     </row>
@@ -1946,8 +1948,8 @@
       <c r="F5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>21</v>
+      <c r="G5" s="21" t="s">
+        <v>272</v>
       </c>
       <c r="H5" s="5"/>
     </row>
@@ -1971,13 +1973,13 @@
         <v>17</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B7" s="16">
         <v>9</v>
@@ -1989,343 +1991,343 @@
         <v>11</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B8" s="16">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="237" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B9" s="16">
         <v>77</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B10" s="16">
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B11" s="16">
         <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="16">
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>31</v>
-      </c>
       <c r="G12" s="6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="16">
         <v>4</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="H13" s="5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="16">
         <v>6</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="16">
         <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="H15" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="16">
         <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="H16" s="5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B17" s="16">
         <v>12</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="16">
         <v>4</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="20" t="s">
         <v>48</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="5" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="16">
         <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="16">
         <v>2</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="G20" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="H20" s="5"/>
     </row>
@@ -2337,676 +2339,674 @@
         <v>1</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="16">
         <v>8</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="16">
         <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="16">
         <v>8</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="16">
         <v>4</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
-        <v>141</v>
+      <c r="A26" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="B26" s="16">
         <v>12</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="16">
         <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B28" s="16">
         <v>1</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B29" s="16">
         <v>11</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="16">
         <v>1</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>88</v>
+        <v>273</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>67</v>
+        <v>191</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>89</v>
+        <v>274</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>219</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="G30" s="21"/>
       <c r="H30" s="5" t="s">
-        <v>170</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="16">
         <v>7</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="E31" s="9" t="s">
+      <c r="F31" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="G31" s="6" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="16">
         <v>7</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B33" s="16">
         <v>13</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B34" s="16">
         <v>24</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="16">
         <v>4</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B36" s="16">
         <v>12</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="16">
         <v>12</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="16">
         <v>2</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B39" s="16">
         <v>2</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B40" s="16">
         <v>52</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B41" s="19">
         <v>4</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B42" s="16">
         <v>1</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="9" t="s">
+      <c r="F42" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="G42" s="6" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="16">
         <v>2</v>
       </c>
       <c r="C43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="9" t="s">
+      <c r="F43" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="G43" s="6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="16">
         <v>1</v>
       </c>
       <c r="C44" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="7" t="s">
+      <c r="F44" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="G44" s="6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="24"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="16">
         <v>1</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="16">
         <v>1</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="24"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="16">
         <v>2</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D47" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H47" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>258</v>
-      </c>
     </row>
     <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="24"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="16">
         <v>1</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="F48" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="H48" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>